<commit_message>
Add chart showing all episodes
- Updated overnight ratings 2024-06-23
- Added page for showing a chart for all episodes (currently overnight only)
- Moved DI registration to AddDoctorWhoCharting extension
- Added icons
- Renamed master assets files
- Removed manual testing data loading
</commit_message>
<xml_diff>
--- a/DoctorWhoRatings.WebClient/wwwroot/data/DoctorWhoRatings.xlsx
+++ b/DoctorWhoRatings.WebClient/wwwroot/data/DoctorWhoRatings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\Personal\GitHubRepos\doctor-who-ratings\DoctorWhoRatings.WebClient\wwwroot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{33C6B3F5-5470-4054-BF97-6F3C07C701DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{A4BC2B24-ED7E-4F1D-94A6-983F713B31C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{79C5864F-570D-459B-A9D3-4650086D0E3E}"/>
   </bookViews>
@@ -2201,9 +2201,9 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97F1EB88-18DF-4495-9368-D4C1B5B3A750}">
   <dimension ref="A1:W887"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A869" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O887" sqref="O887"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -66167,6 +66167,9 @@
       <c r="O885">
         <v>2.11</v>
       </c>
+      <c r="P885">
+        <v>3.18</v>
+      </c>
       <c r="Q885">
         <v>3.52</v>
       </c>
@@ -66174,9 +66177,9 @@
         <f t="shared" si="39"/>
         <v>2.11</v>
       </c>
-      <c r="S885" t="str">
+      <c r="S885">
         <f t="shared" si="40"/>
-        <v/>
+        <v>3.18</v>
       </c>
       <c r="T885">
         <f t="shared" si="41"/>
@@ -66301,9 +66304,12 @@
       <c r="N887" s="6" t="d">
         <v>2024-06-22</v>
       </c>
-      <c r="R887" t="str">
+      <c r="O887">
+        <v>2.25</v>
+      </c>
+      <c r="R887">
         <f t="shared" si="39"/>
-        <v/>
+        <v>2.25</v>
       </c>
       <c r="S887" t="str">
         <f t="shared" si="40"/>

</xml_diff>

<commit_message>
Add chart showing average ratings by doctor
- Added new icons
- Added page for showing a chart for averages grouped by doctor
- Add ability to change calculation based on mean/median and population
</commit_message>
<xml_diff>
--- a/DoctorWhoRatings.WebClient/wwwroot/data/DoctorWhoRatings.xlsx
+++ b/DoctorWhoRatings.WebClient/wwwroot/data/DoctorWhoRatings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\Personal\GitHubRepos\doctor-who-ratings\DoctorWhoRatings.WebClient\wwwroot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{A4BC2B24-ED7E-4F1D-94A6-983F713B31C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0F51D39B-68C4-4CEF-95EF-541ABED6B9AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{79C5864F-570D-459B-A9D3-4650086D0E3E}"/>
   </bookViews>
@@ -2201,9 +2201,9 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97F1EB88-18DF-4495-9368-D4C1B5B3A750}">
   <dimension ref="A1:W887"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A869" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O887" sqref="O887"/>
+      <selection pane="bottomLeft" activeCell="Q886" sqref="Q886"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
Refactor tooltips into smaller components
- Refactored tooltips into smaller components reducing duplication, and allowing reuse via more of a "pick n mix" approach
- Renamed ChartOptionsSet to ChartOptionsGroup
- Updated spreadsheet with latest ratings
</commit_message>
<xml_diff>
--- a/DoctorWhoRatings.WebClient/wwwroot/data/DoctorWhoRatings.xlsx
+++ b/DoctorWhoRatings.WebClient/wwwroot/data/DoctorWhoRatings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\Personal\GitHubRepos\doctor-who-ratings\DoctorWhoRatings.WebClient\wwwroot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{A75BA88B-90D6-4F0C-B0B6-F11822ED903D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{66457E96-9CB0-4FAD-A4C1-C6AC32F06A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{79C5864F-570D-459B-A9D3-4650086D0E3E}"/>
   </bookViews>
@@ -2205,8 +2205,8 @@
   <dimension ref="A1:X887"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A347" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P359" sqref="P359"/>
+      <pane ySplit="1" topLeftCell="A870" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q888" sqref="Q888"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -68969,6 +68969,9 @@
       <c r="P887">
         <v>2.25</v>
       </c>
+      <c r="Q887">
+        <v>3.27</v>
+      </c>
       <c r="R887">
         <v>3.69</v>
       </c>
@@ -68976,9 +68979,9 @@
         <f t="shared" si="39"/>
         <v>2.25</v>
       </c>
-      <c r="T887" t="str">
+      <c r="T887">
         <f t="shared" si="40"/>
-        <v/>
+        <v>3.27</v>
       </c>
       <c r="U887">
         <f t="shared" si="41"/>

</xml_diff>

<commit_message>
Update data for Christmas Special 2024
</commit_message>
<xml_diff>
--- a/DoctorWhoRatings.WebClient/wwwroot/data/DoctorWhoRatings.xlsx
+++ b/DoctorWhoRatings.WebClient/wwwroot/data/DoctorWhoRatings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\Personal\GitHubRepos\doctor-who-ratings\DoctorWhoRatings.WebClient\wwwroot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{FB381018-3D74-4D11-BEDE-14908B86026E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{6233B89A-5552-406A-8ADE-8577C2FBD8A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{79C5864F-570D-459B-A9D3-4650086D0E3E}"/>
   </bookViews>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="2588" uniqueCount="926">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="2590" uniqueCount="928">
   <si>
     <t>Battlefield</t>
   </si>
@@ -2846,6 +2846,12 @@
   </si>
   <si>
     <t>WikiFormatDescription</t>
+  </si>
+  <si>
+    <t>Joy to the World</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Joy_to_the_World_(Doctor_Who)</t>
   </si>
 </sst>
 </file>
@@ -3266,11 +3272,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97F1EB88-18DF-4495-9368-D4C1B5B3A750}">
-  <dimension ref="A1:AC887"/>
+  <dimension ref="A1:AC888"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A684" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AB700" sqref="AB700"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A872" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U888" sqref="U888"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -80335,7 +80341,7 @@
         <v>5.85</v>
       </c>
       <c r="U836">
-        <f t="shared" ref="U836:U887" si="39">IF(ISBLANK(R836),"",ROUND(R836*Y836,2))</f>
+        <f t="shared" ref="U836:U888" si="39">IF(ISBLANK(R836),"",ROUND(R836*Y836,2))</f>
         <v>3.68</v>
       </c>
       <c r="V836">
@@ -85100,6 +85106,87 @@
       </c>
       <c r="AC887" t="s">
         <v>660</v>
+      </c>
+    </row>
+    <row r="888" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A888" s="3">
+        <v>884</v>
+      </c>
+      <c r="B888" s="3">
+        <v>4</v>
+      </c>
+      <c r="C888" s="3" t="str">
+        <f>VLOOKUP(B888,Era!$A$3:$B$999,2,0)</f>
+        <v>New/Disney</v>
+      </c>
+      <c r="D888" s="3">
+        <v>2</v>
+      </c>
+      <c r="E888" s="3" t="str">
+        <f>VLOOKUP(D888,EpisodeFormats!$A$3:$B$999,2,0)</f>
+        <v>Special</v>
+      </c>
+      <c r="F888" s="3">
+        <v>15</v>
+      </c>
+      <c r="G888" s="3" t="str">
+        <f>VLOOKUP(F888,Doctors!$A$3:$B$999,2,0)</f>
+        <v>Ncuti Gatwa</v>
+      </c>
+      <c r="I888" s="3">
+        <v>4</v>
+      </c>
+      <c r="J888" s="3" t="str">
+        <f>VLOOKUP(I888,SeasonFormats!$A$3:$B$999,2,0)</f>
+        <v>Special</v>
+      </c>
+      <c r="K888" s="3">
+        <v>312</v>
+      </c>
+      <c r="M888" s="3" t="s">
+        <v>926</v>
+      </c>
+      <c r="N888" s="3">
+        <v>1</v>
+      </c>
+      <c r="P888" s="7" t="d">
+        <v>2024-12-25</v>
+      </c>
+      <c r="Q888" s="3">
+        <v>55</v>
+      </c>
+      <c r="R888" s="3">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="U888" s="3">
+        <f t="shared" si="39"/>
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="V888" s="3" t="str">
+        <f t="shared" ref="V888" si="42">IF(ISBLANK(S888),"",ROUND(S888*Y888,2))</f>
+        <v/>
+      </c>
+      <c r="W888" s="3" t="str">
+        <f t="shared" ref="W888" si="43">IF(ISBLANK(T888),"",ROUND(T888*Y888,2))</f>
+        <v/>
+      </c>
+      <c r="X888" s="3">
+        <f>VLOOKUP(YEAR(P888),Populations!$A$3:$B$999,2,0)</f>
+        <v>68081792</v>
+      </c>
+      <c r="Y888" s="3">
+        <f>(Calculations!B1/X888)</f>
+        <v>1</v>
+      </c>
+      <c r="AA888" s="3">
+        <v>2</v>
+      </c>
+      <c r="AB888" s="3" t="str">
+        <f>VLOOKUP(AA888,WikiFormats!$A$3:$B$999,2,0)</f>
+        <v>Episode</v>
+      </c>
+      <c r="AC888" s="3" t="s">
+        <v>927</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add filtering on the episode guide page
- Added ability to filter by the story name or episode name
- Needed to restructure the underlying data. For simplicity, the spreadsheet is a very flat structure. This was reflected in the previous code with some metadata for providing formatting information. This doesn't work for a filter as you need to know more about the hierarchy. e.g. The story and episode is on the same row. If a story contains the text but the episode doesn't then you need the row for the story, but then having the row implies the episode is relevant even though it doesn't match. The context is also required, which is only available after the structure is built, and isn't possible with an "as you go" approach
- Implemented new hierarchical structure for above using doctor-season-story-episode
- Season is general term that applies to a group of stories or specials
- Fix a couple of wiki references in the spreadsheet
</commit_message>
<xml_diff>
--- a/DoctorWhoRatings.WebClient/wwwroot/data/DoctorWhoRatings.xlsx
+++ b/DoctorWhoRatings.WebClient/wwwroot/data/DoctorWhoRatings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\Personal\GitHubRepos\doctor-who-ratings\DoctorWhoRatings.WebClient\wwwroot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{818DB60D-F3B7-41C8-A030-F7D336A7377D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{192A1FE6-6C54-4EC6-A2FF-213DE3E96F4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15466" xr2:uid="{79C5864F-570D-459B-A9D3-4650086D0E3E}"/>
+    <workbookView xWindow="5820" yWindow="2547" windowWidth="19200" windowHeight="13066" xr2:uid="{79C5864F-570D-459B-A9D3-4650086D0E3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Episodes" sheetId="2" r:id="rId1"/>
@@ -3274,9 +3274,9 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97F1EB88-18DF-4495-9368-D4C1B5B3A750}">
   <dimension ref="A1:AD888"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E594" sqref="E594"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A595" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AB605" sqref="AB605"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -61191,11 +61191,11 @@
       </c>
       <c r="AA604" s="3"/>
       <c r="AB604" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AC604" s="3" t="str">
         <f>VLOOKUP(AB604,WikiFormats!$A$3:$B$999,2,0)</f>
-        <v>Story</v>
+        <v>Episode</v>
       </c>
       <c r="AD604" s="3" t="s">
         <v>714</v>
@@ -85646,11 +85646,11 @@
         <v>536</v>
       </c>
       <c r="AB866" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AC866" s="3" t="str">
         <f>VLOOKUP(AB866,WikiFormats!$A$3:$B$999,2,0)</f>
-        <v>Story</v>
+        <v>Episode</v>
       </c>
       <c r="AD866" s="3" t="s">
         <v>899</v>

</xml_diff>

<commit_message>
Update Ratings - Overnight - S15E03
</commit_message>
<xml_diff>
--- a/DoctorWhoRatings.WebClient/wwwroot/data/DoctorWhoRatings.xlsx
+++ b/DoctorWhoRatings.WebClient/wwwroot/data/DoctorWhoRatings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\Personal\GitHubRepos\doctor-who-ratings\DoctorWhoRatings.WebClient\wwwroot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{AF3AEAF6-F8ED-4028-A760-05797C75AAAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{4582E634-25C6-417E-B466-154AD23D91A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15466" xr2:uid="{79C5864F-570D-459B-A9D3-4650086D0E3E}"/>
   </bookViews>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="2594" uniqueCount="930">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="2598" uniqueCount="934">
   <si>
     <t>Battlefield</t>
   </si>
@@ -2858,6 +2858,18 @@
   </si>
   <si>
     <t>The Robot Revolution</t>
+  </si>
+  <si>
+    <t>Lux</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Lux_(Doctor_Who)</t>
+  </si>
+  <si>
+    <t>The Well</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/The_Well_(Doctor_Who)</t>
   </si>
 </sst>
 </file>
@@ -3278,11 +3290,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97F1EB88-18DF-4495-9368-D4C1B5B3A750}">
-  <dimension ref="A1:AD889"/>
+  <dimension ref="A1:AD891"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A859" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A889" sqref="A889"/>
+      <pane ySplit="1" topLeftCell="A865" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A891" sqref="A891"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -87791,17 +87803,23 @@
       <c r="S889">
         <v>2</v>
       </c>
+      <c r="T889">
+        <v>3.36</v>
+      </c>
+      <c r="U889">
+        <v>3.57</v>
+      </c>
       <c r="V889">
         <f t="shared" ref="V889" si="44">IF(ISBLANK(S889),"",ROUND(S889*Z889,2))</f>
         <v>2</v>
       </c>
-      <c r="W889" t="str">
+      <c r="W889">
         <f t="shared" si="42"/>
-        <v/>
-      </c>
-      <c r="X889" t="str">
+        <v>3.36</v>
+      </c>
+      <c r="X889">
         <f t="shared" si="43"/>
-        <v/>
+        <v>3.57</v>
       </c>
       <c r="Y889">
         <f>VLOOKUP(YEAR(Q889),Populations!$A$3:$B$999,2,0)</f>
@@ -87820,6 +87838,186 @@
       </c>
       <c r="AD889" t="s">
         <v>928</v>
+      </c>
+    </row>
+    <row r="890" spans="1:30" x14ac:dyDescent="0.5">
+      <c r="A890">
+        <v>886</v>
+      </c>
+      <c r="B890">
+        <v>4</v>
+      </c>
+      <c r="C890" t="str">
+        <f>VLOOKUP(B890,Eras!$A$3:$B$999,2,0)</f>
+        <v>New/Disney</v>
+      </c>
+      <c r="D890">
+        <v>1</v>
+      </c>
+      <c r="E890" t="str">
+        <f>VLOOKUP(D890,EpisodeFormats!$A$3:$B$999,2,0)</f>
+        <v>Series</v>
+      </c>
+      <c r="F890">
+        <v>15</v>
+      </c>
+      <c r="G890" t="str">
+        <f>VLOOKUP(F890,Doctors!$A$3:$B$999,2,0)</f>
+        <v>Ncuti Gatwa</v>
+      </c>
+      <c r="H890">
+        <v>15</v>
+      </c>
+      <c r="I890">
+        <v>3</v>
+      </c>
+      <c r="J890" t="str">
+        <f>VLOOKUP(I890,SeasonFormats!$A$3:$B$999,2,0)</f>
+        <v>Series</v>
+      </c>
+      <c r="K890">
+        <v>314</v>
+      </c>
+      <c r="L890">
+        <v>2</v>
+      </c>
+      <c r="M890" t="s">
+        <v>930</v>
+      </c>
+      <c r="N890">
+        <v>1</v>
+      </c>
+      <c r="P890">
+        <v>1</v>
+      </c>
+      <c r="Q890" s="6" t="d">
+        <v>2025-04-19</v>
+      </c>
+      <c r="R890">
+        <v>44</v>
+      </c>
+      <c r="S890">
+        <v>1.58</v>
+      </c>
+      <c r="V890">
+        <f t="shared" ref="V890" si="45">IF(ISBLANK(S890),"",ROUND(S890*Z890,2))</f>
+        <v>1.58</v>
+      </c>
+      <c r="W890" t="str">
+        <f t="shared" ref="W890" si="46">IF(ISBLANK(T890),"",ROUND(T890*Z890,2))</f>
+        <v/>
+      </c>
+      <c r="X890" t="str">
+        <f t="shared" ref="X890" si="47">IF(ISBLANK(U890),"",ROUND(U890*Z890,2))</f>
+        <v/>
+      </c>
+      <c r="Y890">
+        <f>VLOOKUP(YEAR(Q890),Populations!$A$3:$B$999,2,0)</f>
+        <v>68304932</v>
+      </c>
+      <c r="Z890">
+        <f>(Calculations!B1/Y890)</f>
+        <v>1</v>
+      </c>
+      <c r="AB890">
+        <v>2</v>
+      </c>
+      <c r="AC890" t="str">
+        <f>VLOOKUP(AB890,WikiFormats!$A$3:$B$999,2,0)</f>
+        <v>Episode</v>
+      </c>
+      <c r="AD890" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="891" spans="1:30" x14ac:dyDescent="0.5">
+      <c r="A891">
+        <v>887</v>
+      </c>
+      <c r="B891">
+        <v>4</v>
+      </c>
+      <c r="C891" t="str">
+        <f>VLOOKUP(B891,Eras!$A$3:$B$999,2,0)</f>
+        <v>New/Disney</v>
+      </c>
+      <c r="D891">
+        <v>1</v>
+      </c>
+      <c r="E891" t="str">
+        <f>VLOOKUP(D891,EpisodeFormats!$A$3:$B$999,2,0)</f>
+        <v>Series</v>
+      </c>
+      <c r="F891">
+        <v>15</v>
+      </c>
+      <c r="G891" t="str">
+        <f>VLOOKUP(F891,Doctors!$A$3:$B$999,2,0)</f>
+        <v>Ncuti Gatwa</v>
+      </c>
+      <c r="H891">
+        <v>15</v>
+      </c>
+      <c r="I891">
+        <v>3</v>
+      </c>
+      <c r="J891" t="str">
+        <f>VLOOKUP(I891,SeasonFormats!$A$3:$B$999,2,0)</f>
+        <v>Series</v>
+      </c>
+      <c r="K891">
+        <v>315</v>
+      </c>
+      <c r="L891">
+        <v>3</v>
+      </c>
+      <c r="M891" t="s">
+        <v>932</v>
+      </c>
+      <c r="N891">
+        <v>1</v>
+      </c>
+      <c r="P891">
+        <v>1</v>
+      </c>
+      <c r="Q891" s="6" t="d">
+        <v>2025-04-26</v>
+      </c>
+      <c r="R891">
+        <v>48</v>
+      </c>
+      <c r="S891">
+        <v>1.86</v>
+      </c>
+      <c r="V891">
+        <f t="shared" ref="V891" si="48">IF(ISBLANK(S891),"",ROUND(S891*Z891,2))</f>
+        <v>1.86</v>
+      </c>
+      <c r="W891" t="str">
+        <f t="shared" ref="W891" si="49">IF(ISBLANK(T891),"",ROUND(T891*Z891,2))</f>
+        <v/>
+      </c>
+      <c r="X891" t="str">
+        <f t="shared" ref="X891" si="50">IF(ISBLANK(U891),"",ROUND(U891*Z891,2))</f>
+        <v/>
+      </c>
+      <c r="Y891">
+        <f>VLOOKUP(YEAR(Q891),Populations!$A$3:$B$999,2,0)</f>
+        <v>68304932</v>
+      </c>
+      <c r="Z891">
+        <f>(Calculations!B1/Y891)</f>
+        <v>1</v>
+      </c>
+      <c r="AB891">
+        <v>2</v>
+      </c>
+      <c r="AC891" t="str">
+        <f>VLOOKUP(AB891,WikiFormats!$A$3:$B$999,2,0)</f>
+        <v>Episode</v>
+      </c>
+      <c r="AD891" t="s">
+        <v>933</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Ratings - Extended - S15E02
</commit_message>
<xml_diff>
--- a/DoctorWhoRatings.WebClient/wwwroot/data/DoctorWhoRatings.xlsx
+++ b/DoctorWhoRatings.WebClient/wwwroot/data/DoctorWhoRatings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\Personal\GitHubRepos\doctor-who-ratings\DoctorWhoRatings.WebClient\wwwroot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{4582E634-25C6-417E-B466-154AD23D91A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{3BF08FB7-D3EF-43DB-81F2-30FEE3DED0F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15466" xr2:uid="{79C5864F-570D-459B-A9D3-4650086D0E3E}"/>
   </bookViews>
@@ -3292,9 +3292,9 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97F1EB88-18DF-4495-9368-D4C1B5B3A750}">
   <dimension ref="A1:AD891"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A865" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A891" sqref="A891"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A868" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U891" sqref="U891"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -87899,6 +87899,9 @@
       <c r="S890">
         <v>1.58</v>
       </c>
+      <c r="U890">
+        <v>3</v>
+      </c>
       <c r="V890">
         <f t="shared" ref="V890" si="45">IF(ISBLANK(S890),"",ROUND(S890*Z890,2))</f>
         <v>1.58</v>
@@ -87907,9 +87910,9 @@
         <f t="shared" ref="W890" si="46">IF(ISBLANK(T890),"",ROUND(T890*Z890,2))</f>
         <v/>
       </c>
-      <c r="X890" t="str">
+      <c r="X890">
         <f t="shared" ref="X890" si="47">IF(ISBLANK(U890),"",ROUND(U890*Z890,2))</f>
-        <v/>
+        <v>3</v>
       </c>
       <c r="Y890">
         <f>VLOOKUP(YEAR(Q890),Populations!$A$3:$B$999,2,0)</f>

</xml_diff>

<commit_message>
Update ratings - Consolidated - S15E02
</commit_message>
<xml_diff>
--- a/DoctorWhoRatings.WebClient/wwwroot/data/DoctorWhoRatings.xlsx
+++ b/DoctorWhoRatings.WebClient/wwwroot/data/DoctorWhoRatings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\Personal\GitHubRepos\doctor-who-ratings\DoctorWhoRatings.WebClient\wwwroot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{3BF08FB7-D3EF-43DB-81F2-30FEE3DED0F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{DF2105AD-7214-4A26-927E-054DCF08A177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15466" xr2:uid="{79C5864F-570D-459B-A9D3-4650086D0E3E}"/>
   </bookViews>
@@ -3294,7 +3294,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A868" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U891" sqref="U891"/>
+      <selection pane="bottomLeft" activeCell="T891" sqref="T891"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -87899,6 +87899,9 @@
       <c r="S890">
         <v>1.58</v>
       </c>
+      <c r="T890">
+        <v>2.69</v>
+      </c>
       <c r="U890">
         <v>3</v>
       </c>
@@ -87906,9 +87909,9 @@
         <f t="shared" ref="V890" si="45">IF(ISBLANK(S890),"",ROUND(S890*Z890,2))</f>
         <v>1.58</v>
       </c>
-      <c r="W890" t="str">
+      <c r="W890">
         <f t="shared" ref="W890" si="46">IF(ISBLANK(T890),"",ROUND(T890*Z890,2))</f>
-        <v/>
+        <v>2.69</v>
       </c>
       <c r="X890">
         <f t="shared" ref="X890" si="47">IF(ISBLANK(U890),"",ROUND(U890*Z890,2))</f>

</xml_diff>

<commit_message>
Update ratings - Overnight - S15E04
</commit_message>
<xml_diff>
--- a/DoctorWhoRatings.WebClient/wwwroot/data/DoctorWhoRatings.xlsx
+++ b/DoctorWhoRatings.WebClient/wwwroot/data/DoctorWhoRatings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\Personal\GitHubRepos\doctor-who-ratings\DoctorWhoRatings.WebClient\wwwroot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{DF2105AD-7214-4A26-927E-054DCF08A177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0F66B23E-06E6-4A63-81EB-7718CFC7A232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15466" xr2:uid="{79C5864F-570D-459B-A9D3-4650086D0E3E}"/>
   </bookViews>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="2598" uniqueCount="934">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="2600" uniqueCount="936">
   <si>
     <t>Battlefield</t>
   </si>
@@ -2870,6 +2870,12 @@
   </si>
   <si>
     <t>https://en.wikipedia.org/wiki/The_Well_(Doctor_Who)</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Lucky_Day_(Doctor_Who)</t>
+  </si>
+  <si>
+    <t>Lucky Day</t>
   </si>
 </sst>
 </file>
@@ -3290,11 +3296,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97F1EB88-18DF-4495-9368-D4C1B5B3A750}">
-  <dimension ref="A1:AD891"/>
+  <dimension ref="A1:AD892"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A868" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T891" sqref="T891"/>
+      <selection pane="bottomLeft" activeCell="J892" sqref="J892"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -88026,6 +88032,96 @@
         <v>933</v>
       </c>
     </row>
+    <row r="892" spans="1:30" x14ac:dyDescent="0.5">
+      <c r="A892">
+        <v>888</v>
+      </c>
+      <c r="B892">
+        <v>4</v>
+      </c>
+      <c r="C892" t="str">
+        <f>VLOOKUP(B892,Eras!$A$3:$B$999,2,0)</f>
+        <v>New/Disney</v>
+      </c>
+      <c r="D892">
+        <v>1</v>
+      </c>
+      <c r="E892" t="str">
+        <f>VLOOKUP(D892,EpisodeFormats!$A$3:$B$999,2,0)</f>
+        <v>Series</v>
+      </c>
+      <c r="F892">
+        <v>15</v>
+      </c>
+      <c r="G892" t="str">
+        <f>VLOOKUP(F892,Doctors!$A$3:$B$999,2,0)</f>
+        <v>Ncuti Gatwa</v>
+      </c>
+      <c r="H892">
+        <v>15</v>
+      </c>
+      <c r="I892">
+        <v>3</v>
+      </c>
+      <c r="J892" t="str">
+        <f>VLOOKUP(I892,SeasonFormats!$A$3:$B$999,2,0)</f>
+        <v>Series</v>
+      </c>
+      <c r="K892">
+        <v>316</v>
+      </c>
+      <c r="L892">
+        <v>4</v>
+      </c>
+      <c r="M892" t="s">
+        <v>935</v>
+      </c>
+      <c r="N892">
+        <v>1</v>
+      </c>
+      <c r="P892">
+        <v>1</v>
+      </c>
+      <c r="Q892" s="6" t="d">
+        <v>2025-05-03</v>
+      </c>
+      <c r="R892">
+        <v>46</v>
+      </c>
+      <c r="S892">
+        <v>1.5</v>
+      </c>
+      <c r="V892">
+        <f t="shared" ref="V892" si="51">IF(ISBLANK(S892),"",ROUND(S892*Z892,2))</f>
+        <v>1.5</v>
+      </c>
+      <c r="W892" t="str">
+        <f t="shared" ref="W892" si="52">IF(ISBLANK(T892),"",ROUND(T892*Z892,2))</f>
+        <v/>
+      </c>
+      <c r="X892" t="str">
+        <f t="shared" ref="X892" si="53">IF(ISBLANK(U892),"",ROUND(U892*Z892,2))</f>
+        <v/>
+      </c>
+      <c r="Y892">
+        <f>VLOOKUP(YEAR(Q892),Populations!$A$3:$B$999,2,0)</f>
+        <v>68304932</v>
+      </c>
+      <c r="Z892">
+        <f>(Calculations!B1/Y892)</f>
+        <v>1</v>
+      </c>
+      <c r="AB892">
+        <v>2</v>
+      </c>
+      <c r="AC892" t="str">
+        <f>VLOOKUP(AB892,WikiFormats!$A$3:$B$999,2,0)</f>
+        <v>Episode</v>
+      </c>
+      <c r="AD892" t="s">
+        <v>934</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update ratings - Consolidated/Extended- S15E04
</commit_message>
<xml_diff>
--- a/DoctorWhoRatings.WebClient/wwwroot/data/DoctorWhoRatings.xlsx
+++ b/DoctorWhoRatings.WebClient/wwwroot/data/DoctorWhoRatings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\Personal\GitHubRepos\doctor-who-ratings\DoctorWhoRatings.WebClient\wwwroot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0F66B23E-06E6-4A63-81EB-7718CFC7A232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{CD0313E1-45DD-4E32-9F85-1346DD4684FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15466" xr2:uid="{79C5864F-570D-459B-A9D3-4650086D0E3E}"/>
   </bookViews>
@@ -3298,9 +3298,9 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97F1EB88-18DF-4495-9368-D4C1B5B3A750}">
   <dimension ref="A1:AD892"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A868" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J892" sqref="J892"/>
+      <selection pane="bottomLeft" activeCell="T892" sqref="T892"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -88001,17 +88001,23 @@
       <c r="S891">
         <v>1.86</v>
       </c>
+      <c r="T891">
+        <v>2.91</v>
+      </c>
+      <c r="U891">
+        <v>3.23</v>
+      </c>
       <c r="V891">
         <f t="shared" ref="V891" si="48">IF(ISBLANK(S891),"",ROUND(S891*Z891,2))</f>
         <v>1.86</v>
       </c>
-      <c r="W891" t="str">
+      <c r="W891">
         <f t="shared" ref="W891" si="49">IF(ISBLANK(T891),"",ROUND(T891*Z891,2))</f>
-        <v/>
-      </c>
-      <c r="X891" t="str">
+        <v>2.91</v>
+      </c>
+      <c r="X891">
         <f t="shared" ref="X891" si="50">IF(ISBLANK(U891),"",ROUND(U891*Z891,2))</f>
-        <v/>
+        <v>3.23</v>
       </c>
       <c r="Y891">
         <f>VLOOKUP(YEAR(Q891),Populations!$A$3:$B$999,2,0)</f>

</xml_diff>

<commit_message>
Update ratings - S15E06 overnights and E05 consolidated
</commit_message>
<xml_diff>
--- a/DoctorWhoRatings.WebClient/wwwroot/data/DoctorWhoRatings.xlsx
+++ b/DoctorWhoRatings.WebClient/wwwroot/data/DoctorWhoRatings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\Personal\GitHubRepos\doctor-who-ratings\DoctorWhoRatings.WebClient\wwwroot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{CD0313E1-45DD-4E32-9F85-1346DD4684FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0AC82992-5C34-484A-8D5D-D46F6B970992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15466" xr2:uid="{79C5864F-570D-459B-A9D3-4650086D0E3E}"/>
   </bookViews>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="2600" uniqueCount="936">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="2604" uniqueCount="940">
   <si>
     <t>Battlefield</t>
   </si>
@@ -2876,6 +2876,18 @@
   </si>
   <si>
     <t>Lucky Day</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/The_Story_%26_the_Engine</t>
+  </si>
+  <si>
+    <t>The Story and the Engine</t>
+  </si>
+  <si>
+    <t>The Interstellar Song Contest</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/The_Interstellar_Song_Contest</t>
   </si>
 </sst>
 </file>
@@ -3296,11 +3308,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97F1EB88-18DF-4495-9368-D4C1B5B3A750}">
-  <dimension ref="A1:AD892"/>
+  <dimension ref="A1:AD894"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A868" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T892" sqref="T892"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A870" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U894" sqref="U894"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -87894,7 +87906,7 @@
         <v>1</v>
       </c>
       <c r="P890">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q890" s="6" t="d">
         <v>2025-04-19</v>
@@ -87990,7 +88002,7 @@
         <v>1</v>
       </c>
       <c r="P891">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q891" s="6" t="d">
         <v>2025-04-26</v>
@@ -88086,7 +88098,7 @@
         <v>1</v>
       </c>
       <c r="P892">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Q892" s="6" t="d">
         <v>2025-05-03</v>
@@ -88096,18 +88108,24 @@
       </c>
       <c r="S892">
         <v>1.5</v>
+      </c>
+      <c r="T892">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="U892">
+        <v>2.8</v>
       </c>
       <c r="V892">
         <f t="shared" ref="V892" si="51">IF(ISBLANK(S892),"",ROUND(S892*Z892,2))</f>
         <v>1.5</v>
       </c>
-      <c r="W892" t="str">
+      <c r="W892">
         <f t="shared" ref="W892" si="52">IF(ISBLANK(T892),"",ROUND(T892*Z892,2))</f>
-        <v/>
-      </c>
-      <c r="X892" t="str">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="X892">
         <f t="shared" ref="X892" si="53">IF(ISBLANK(U892),"",ROUND(U892*Z892,2))</f>
-        <v/>
+        <v>2.8</v>
       </c>
       <c r="Y892">
         <f>VLOOKUP(YEAR(Q892),Populations!$A$3:$B$999,2,0)</f>
@@ -88126,6 +88144,192 @@
       </c>
       <c r="AD892" t="s">
         <v>934</v>
+      </c>
+    </row>
+    <row r="893" spans="1:30" x14ac:dyDescent="0.5">
+      <c r="A893">
+        <v>889</v>
+      </c>
+      <c r="B893">
+        <v>4</v>
+      </c>
+      <c r="C893" t="str">
+        <f>VLOOKUP(B893,Eras!$A$3:$B$999,2,0)</f>
+        <v>New/Disney</v>
+      </c>
+      <c r="D893">
+        <v>1</v>
+      </c>
+      <c r="E893" t="str">
+        <f>VLOOKUP(D893,EpisodeFormats!$A$3:$B$999,2,0)</f>
+        <v>Series</v>
+      </c>
+      <c r="F893">
+        <v>15</v>
+      </c>
+      <c r="G893" t="str">
+        <f>VLOOKUP(F893,Doctors!$A$3:$B$999,2,0)</f>
+        <v>Ncuti Gatwa</v>
+      </c>
+      <c r="H893">
+        <v>15</v>
+      </c>
+      <c r="I893">
+        <v>3</v>
+      </c>
+      <c r="J893" t="str">
+        <f>VLOOKUP(I893,SeasonFormats!$A$3:$B$999,2,0)</f>
+        <v>Series</v>
+      </c>
+      <c r="K893">
+        <v>317</v>
+      </c>
+      <c r="L893">
+        <v>5</v>
+      </c>
+      <c r="M893" t="s">
+        <v>937</v>
+      </c>
+      <c r="N893">
+        <v>1</v>
+      </c>
+      <c r="P893">
+        <v>5</v>
+      </c>
+      <c r="Q893" s="6" t="d">
+        <v>2025-05-10</v>
+      </c>
+      <c r="R893">
+        <v>47</v>
+      </c>
+      <c r="S893">
+        <v>1.59</v>
+      </c>
+      <c r="T893">
+        <v>2.46</v>
+      </c>
+      <c r="U893">
+        <v>2.7</v>
+      </c>
+      <c r="V893">
+        <f t="shared" ref="V893" si="54">IF(ISBLANK(S893),"",ROUND(S893*Z893,2))</f>
+        <v>1.59</v>
+      </c>
+      <c r="W893">
+        <f t="shared" ref="W893" si="55">IF(ISBLANK(T893),"",ROUND(T893*Z893,2))</f>
+        <v>2.46</v>
+      </c>
+      <c r="X893">
+        <f t="shared" ref="X893" si="56">IF(ISBLANK(U893),"",ROUND(U893*Z893,2))</f>
+        <v>2.7</v>
+      </c>
+      <c r="Y893">
+        <f>VLOOKUP(YEAR(Q893),Populations!$A$3:$B$999,2,0)</f>
+        <v>68304932</v>
+      </c>
+      <c r="Z893">
+        <f>(Calculations!B1/Y893)</f>
+        <v>1</v>
+      </c>
+      <c r="AB893">
+        <v>2</v>
+      </c>
+      <c r="AC893" t="str">
+        <f>VLOOKUP(AB893,WikiFormats!$A$3:$B$999,2,0)</f>
+        <v>Episode</v>
+      </c>
+      <c r="AD893" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="894" spans="1:30" x14ac:dyDescent="0.5">
+      <c r="A894">
+        <v>890</v>
+      </c>
+      <c r="B894">
+        <v>4</v>
+      </c>
+      <c r="C894" t="str">
+        <f>VLOOKUP(B894,Eras!$A$3:$B$999,2,0)</f>
+        <v>New/Disney</v>
+      </c>
+      <c r="D894">
+        <v>1</v>
+      </c>
+      <c r="E894" t="str">
+        <f>VLOOKUP(D894,EpisodeFormats!$A$3:$B$999,2,0)</f>
+        <v>Series</v>
+      </c>
+      <c r="F894">
+        <v>15</v>
+      </c>
+      <c r="G894" t="str">
+        <f>VLOOKUP(F894,Doctors!$A$3:$B$999,2,0)</f>
+        <v>Ncuti Gatwa</v>
+      </c>
+      <c r="H894">
+        <v>15</v>
+      </c>
+      <c r="I894">
+        <v>3</v>
+      </c>
+      <c r="J894" t="str">
+        <f>VLOOKUP(I894,SeasonFormats!$A$3:$B$999,2,0)</f>
+        <v>Series</v>
+      </c>
+      <c r="K894">
+        <v>318</v>
+      </c>
+      <c r="L894">
+        <v>6</v>
+      </c>
+      <c r="M894" t="s">
+        <v>938</v>
+      </c>
+      <c r="N894">
+        <v>1</v>
+      </c>
+      <c r="P894">
+        <v>6</v>
+      </c>
+      <c r="Q894" s="6" t="d">
+        <v>2025-05-17</v>
+      </c>
+      <c r="R894">
+        <v>47</v>
+      </c>
+      <c r="S894">
+        <v>2.57</v>
+      </c>
+      <c r="V894">
+        <f t="shared" ref="V894" si="57">IF(ISBLANK(S894),"",ROUND(S894*Z894,2))</f>
+        <v>2.57</v>
+      </c>
+      <c r="W894" t="str">
+        <f t="shared" ref="W894" si="58">IF(ISBLANK(T894),"",ROUND(T894*Z894,2))</f>
+        <v/>
+      </c>
+      <c r="X894" t="str">
+        <f t="shared" ref="X894" si="59">IF(ISBLANK(U894),"",ROUND(U894*Z894,2))</f>
+        <v/>
+      </c>
+      <c r="Y894">
+        <f>VLOOKUP(YEAR(Q894),Populations!$A$3:$B$999,2,0)</f>
+        <v>68304932</v>
+      </c>
+      <c r="Z894">
+        <f>(Calculations!B1/Y894)</f>
+        <v>1</v>
+      </c>
+      <c r="AB894">
+        <v>2</v>
+      </c>
+      <c r="AC894" t="str">
+        <f>VLOOKUP(AB894,WikiFormats!$A$3:$B$999,2,0)</f>
+        <v>Episode</v>
+      </c>
+      <c r="AD894" t="s">
+        <v>939</v>
       </c>
     </row>
   </sheetData>

</xml_diff>